<commit_message>
added some beats to the beatchart
</commit_message>
<xml_diff>
--- a/beatchart.xlsx
+++ b/beatchart.xlsx
@@ -1,13 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Magic Mike\Desktop\Master\modding y diseño de nivel\Practica-Final-Creacion-de-niveles\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D9A86F7-EB97-4473-80C0-BED2A3A826F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="City Outskirts" sheetId="1" r:id="rId1"/>
+    <sheet name="Red district" sheetId="5" r:id="rId2"/>
+    <sheet name="Higher Echelon (white district)" sheetId="7" r:id="rId3"/>
+    <sheet name="Techno District" sheetId="8" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,9 +27,302 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="64">
+  <si>
+    <t>Game: Elementor;  Level: city outskirts (dark level).</t>
+  </si>
+  <si>
+    <t>Objectives:</t>
+  </si>
+  <si>
+    <t>obtain the dash ability</t>
+  </si>
+  <si>
+    <t>unlock one of the key items for the final level 
+(requires all abilities from other levels)</t>
+  </si>
+  <si>
+    <t>Secondary objective:</t>
+  </si>
+  <si>
+    <t>Main Area:</t>
+  </si>
+  <si>
+    <t>Zone enemies:</t>
+  </si>
+  <si>
+    <t>City Streets - dimly light streets filled with unsanitary waste and
+bad living conditions, poor people and the bad seeds that prey on
+them find themselves here.</t>
+  </si>
+  <si>
+    <t>Zone pickups:</t>
+  </si>
+  <si>
+    <t>Sub-area 1</t>
+  </si>
+  <si>
+    <t>Swamp things, hobos.</t>
+  </si>
+  <si>
+    <t>Sub-area 2</t>
+  </si>
+  <si>
+    <t>Sub - area 3</t>
+  </si>
+  <si>
+    <t>Sewers - access via a destructible wall, the zone has various paths
+that end up merging or in a dead end, kinda laberinticall with constantly respawning enemies. There is a bigger variant of these enemies that block a path to sub area 3, these enemies can only be defeated with the parry attack. can access sub area 2 again from here.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Undergroung bridge - requires dash to cross some water, access to sub area 2 behind a destructible surface ( bomb ability ), can go back to main area from here.
+</t>
+  </si>
+  <si>
+    <t>Animated trash bags,
+tunnel trash door, rat pack</t>
+  </si>
+  <si>
+    <t>Water treatment facility - accesed by defeating the Tunnel trash door. Puzzle platformer that rises to the top from the machining room all while trying to avoid security, you can access the upper spire (sub area 4) with a double jump.</t>
+  </si>
+  <si>
+    <t>Sub - area 4</t>
+  </si>
+  <si>
+    <t>Security guards, water elementals</t>
+  </si>
+  <si>
+    <t>bombs x 3</t>
+  </si>
+  <si>
+    <t>extra life, health refill (1), 3 bullets(1).</t>
+  </si>
+  <si>
+    <t>Water elementals, Leviathan.</t>
+  </si>
+  <si>
+    <t>Upper spire - enter by double jumping , zone contains a boss enemy and can only be defeated if all abilities are used.</t>
+  </si>
+  <si>
+    <t>Street thugs, hobos, junkies, 
+electricians, contruction workers.</t>
+  </si>
+  <si>
+    <t>health pickups (3) , 3 bullets (5)</t>
+  </si>
+  <si>
+    <t>extra life, Water Orb (key item).</t>
+  </si>
+  <si>
+    <t>Zone aesthetics</t>
+  </si>
+  <si>
+    <t>dark tones with yellowish light</t>
+  </si>
+  <si>
+    <t>extra-area-1</t>
+  </si>
+  <si>
+    <t>Rooftops, eneterd by double jumping up some side ladders.</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>bullets  &amp; health.</t>
+  </si>
+  <si>
+    <t>bombs x 5 (2), health refill (1),
+ 3-bullets (2).</t>
+  </si>
+  <si>
+    <t>even darker with fluorescent faded 
+lights from the top of the bridge</t>
+  </si>
+  <si>
+    <t>Dim lighting with fluorescent lights and
+greenish atmosphere to represent the 
+foul smell.</t>
+  </si>
+  <si>
+    <t>cleaner atmosphere more white tones
+and homogenous white light as to
+represent a more streamlined area.</t>
+  </si>
+  <si>
+    <t>continuing the themes of the previous
+zone it contains a lot of running water
+as to give way to the leviathan boss fight.</t>
+  </si>
+  <si>
+    <t>it mantains the aesthetic of the main
+area but with dimmer light since we
+are far away from the streetlights</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">obtain the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dash</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ability</t>
+    </r>
+  </si>
+  <si>
+    <t>Storyline</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">obtain the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>parry</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ability</t>
+    </r>
+  </si>
+  <si>
+    <t>Game: Elementor;  Level: Red district</t>
+  </si>
+  <si>
+    <t>busy boulevard - futuristic district where everything wants to make you enter into their questionable shops, red neon signs everywhere as far as the eye can see. Smoke coming out of the ventilation holes and allis busy with high end cars.</t>
+  </si>
+  <si>
+    <t>red lights... everywhere.</t>
+  </si>
+  <si>
+    <t>gang member, sex worker, pimp, drug
+dealer, club bouncer.</t>
+  </si>
+  <si>
+    <t>blinking multi coloured lights and pink
+aesthetic.</t>
+  </si>
+  <si>
+    <t>partygoer, drunk fighter, DJ.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">private club - requires parry to defeat a club bouncer that the lets
+you inside the most elite club in the city you can exit to the main zone through the backdoor, when u go to the VIP after defeating the DJ you can cross a broken bridge that connects the club to other building with the DASH  &amp; DOUBLE JUMP abilities, finally u open the door with the bombs, or are forced to jump down to the streets again.
+</t>
+  </si>
+  <si>
+    <t>money launderers - the club was only a facade, after crossing the broken bridge we see the place ridden with gangsters and money everywhere, they surely keep the keystone here. You need to all your abilities to progress throught the mobsters and defeat the Mafia family head, Kiyoshiro.</t>
+  </si>
+  <si>
+    <t>mobster (gun), mobster(bat), mobster(katana), Kyoshiro.</t>
+  </si>
+  <si>
+    <t>semi ofice-like building with obvious hints to illegal activity, and some lighting which is questionable, themes of japanese lore plastered all over.</t>
+  </si>
+  <si>
+    <t>extra-area-2</t>
+  </si>
+  <si>
+    <t>back alleys, using a bomb attack to break a destructible wall.</t>
+  </si>
+  <si>
+    <t>Rooftops using double jumps again gets us to the rooftops.</t>
+  </si>
+  <si>
+    <t>same as main area + partygoers.</t>
+  </si>
+  <si>
+    <t>same as main area</t>
+  </si>
+  <si>
+    <t>Somewhere within the red district there is an artifact that  its said could defy time itself, for a short period of time, 
+you require this artifact to get past some of the towers defenses to get to the floor where "Name here" is meant to be. You can also pick up an object guarded by the mafia its said to be able to hold the elemental orbs.</t>
+  </si>
+  <si>
+    <t>Hidden in the outskirts of the city there is a techno suit guarded by the thugs of the mishiva clan, they are tasked
+to guard them but you have other plans. You need this suit to get to the high tower of the evil tyrant "Name Here".
+You've also heard about a magial artifact guarded by a an ancient creature and something about the water treatment facility?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">obtain the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Double Jump</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> ability</t>
+    </r>
+  </si>
+  <si>
+    <t>NAMECORP owned by "Name Here" must be stopped you need to infiltrate into this branch and retrieve the SENPU
+boots, they will help inmensely in your infiltration allowing a brief moment to "step" on the air while jumping.
+You must also get the fire orb, that lies somewhere in...</t>
+  </si>
+  <si>
+    <t>Security guard(plasma gun), security guard(saber baton), robo-guardian</t>
+  </si>
+  <si>
+    <t xml:space="preserve">streets are just average metropolis streets with everything getting much more cable heavy and futuristic the closer you get to the main building. </t>
+  </si>
+  <si>
+    <t>commercial streets - going through a busy urban area, full of people and in the daytime to explore the outside of the building you will be later infiltrating you're spotted by security and promptly chased, you make your escape into the building and are now trying to escape from security while also tracking down the Jump boots. once inside the building you can go into the elevator shaft with and explosion and climb with double jump to access the second floor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">second floor.
+</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,13 +330,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -46,13 +377,33 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="20% - Énfasis2" xfId="2" builtinId="34"/>
+    <cellStyle name="Encabezado 4" xfId="1" builtinId="19"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -330,13 +681,673 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="2" max="2" width="54.44140625" customWidth="1"/>
+    <col min="3" max="9" width="32" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:8" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="109.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C2:E2"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA8A42DA-87BB-4C87-8080-71131A25A378}">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="2" max="2" width="54.44140625" customWidth="1"/>
+    <col min="3" max="9" width="32" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:8" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="109.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="50.4" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FCCF5DC-2441-48EA-B594-63C1673D3296}">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="2" max="2" width="54.44140625" customWidth="1"/>
+    <col min="3" max="9" width="32" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+    </row>
+    <row r="3" spans="1:8" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="123.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="109.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="C2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68D7D466-CDB6-44BF-9716-D5B1BC9E122F}">
+  <dimension ref="A1:H11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="2" max="2" width="54.44140625" customWidth="1"/>
+    <col min="3" max="9" width="32" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="2"/>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
+    </row>
+    <row r="3" spans="1:8" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="110.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="109.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:8" ht="14.4" customHeight="1" x14ac:dyDescent="0.3"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:B1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>